<commit_message>
Started writing initial plan
</commit_message>
<xml_diff>
--- a/doc/log.xlsx
+++ b/doc/log.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Who?</t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t>2h</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Started initial plan</t>
+  </si>
+  <si>
+    <t>Added project context</t>
+  </si>
+  <si>
+    <t>1h</t>
   </si>
 </sst>
 </file>
@@ -198,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -209,6 +221,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -219,11 +234,13 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
         <vertical style="thin">
           <color indexed="64"/>
         </vertical>
@@ -235,21 +252,17 @@
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right/>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
         <bottom style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -324,6 +337,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -338,28 +367,14 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
   </dxfs>
@@ -368,13 +383,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D48" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
-  <autoFilter ref="A1:D48"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E48" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="A1:E48"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="Who?" dataDxfId="4"/>
     <tableColumn id="2" name="Task" dataDxfId="3"/>
     <tableColumn id="3" name="Notes" dataDxfId="2"/>
-    <tableColumn id="4" name="Time spent" dataDxfId="1"/>
+    <tableColumn id="7" name="Date" dataDxfId="1"/>
+    <tableColumn id="4" name="Time spent" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -702,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -714,10 +730,10 @@
     <col min="2" max="2" width="40.6640625" customWidth="1"/>
     <col min="3" max="3" width="65.83203125" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" customWidth="1"/>
-    <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -728,13 +744,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -744,294 +763,353 @@
       <c r="C2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="10">
+        <v>14.3</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
-    </row>
-    <row r="4" spans="1:6">
+    <row r="3" spans="1:7">
+      <c r="A3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="8">
+        <v>14.3</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="8"/>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="6"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="8"/>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="8"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="8"/>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="2"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="8"/>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="8"/>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="8"/>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="8"/>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="2"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="6"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="6"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="6"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="8"/>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="6"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="8"/>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="6"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="8"/>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="6"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="8"/>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="6"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="8"/>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30" s="8"/>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="6"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="8"/>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="6"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="8"/>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="6"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="8"/>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="6"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="8"/>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34" s="8"/>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="6"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
       <c r="D35" s="8"/>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="6"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="8"/>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36" s="8"/>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="2"/>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
       <c r="D37" s="1"/>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="6"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="8"/>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38" s="8"/>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="6"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="8"/>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39" s="8"/>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="6"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="8"/>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40" s="8"/>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="6"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="8"/>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E41" s="8"/>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="6"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="8"/>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="E42" s="8"/>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" s="6"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="8"/>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="E43" s="8"/>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="6"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
       <c r="D44" s="8"/>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="E44" s="8"/>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" s="6"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="8"/>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="E45" s="8"/>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" s="6"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="8"/>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="E46" s="8"/>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" s="6"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="8"/>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="E47" s="8"/>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" s="2"/>
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
       <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
-      <formula1>$F$1:$F$2</formula1>
+      <formula1>$G$1:$G$2</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added README to code folder and updated log
</commit_message>
<xml_diff>
--- a/doc/log.xlsx
+++ b/doc/log.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Who?</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Initial plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setup project infrastructure </t>
+  </si>
+  <si>
+    <t>Created code folder and structur. Added small demo script.</t>
   </si>
 </sst>
 </file>
@@ -727,7 +733,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -814,11 +820,21 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="A5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="8">
+        <v>17.3</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="6"/>

</xml_diff>

<commit_message>
Initial plan:   - Filled the sections Project organization, Constraints and elements of risks and the Deliverables goods   - Added the work to the logbook
</commit_message>
<xml_diff>
--- a/doc/log.xlsx
+++ b/doc/log.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-120" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-120" windowWidth="25600" windowHeight="15100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>Who?</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>Created code folder and structur. Added small demo script.</t>
+  </si>
+  <si>
+    <t>Introduction to video processing with Matlab</t>
+  </si>
+  <si>
+    <t>Started to learn how to process videos with Matlab</t>
+  </si>
+  <si>
+    <t>Added: project organization, constraints &amp; elem of risks and deliverables parts</t>
   </si>
 </sst>
 </file>
@@ -733,7 +742,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -837,18 +846,38 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="A6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="8">
+        <v>17.3</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="A7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="8">
+        <v>19.3</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="6"/>

</xml_diff>